<commit_message>
Added data provider for Cruises Test
</commit_message>
<xml_diff>
--- a/TripAdvisorAutomation/resources/testdata/TestData.xlsx
+++ b/TripAdvisorAutomation/resources/testdata/TestData.xlsx
@@ -3,17 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4830BDE4-74A3-4C90-9995-D649182A5BE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cognizant\Learning\git2\TripAdvisorAutomation\TripAdvisorAutomation\resources\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42E25C7-27F4-479F-91DD-CA4974EBE2BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17304" windowHeight="12312" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3168" yWindow="3168" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
     <sheet name="HolidayHomesTest" sheetId="2" r:id="rId2"/>
     <sheet name="CruisesTest" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:P17"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,69 +27,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>hariniharika12@gmail.com</t>
-  </si>
-  <si>
-    <t>tripadvisorpass</t>
-  </si>
-  <si>
-    <t>Valid credentials</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>dummyemail</t>
-  </si>
-  <si>
-    <t>dummypass</t>
-  </si>
-  <si>
-    <t>Invalid credentials</t>
-  </si>
-  <si>
-    <t>Invalid password</t>
-  </si>
-  <si>
-    <t>Email field empty</t>
-  </si>
-  <si>
-    <t>Password field empty</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Location</t>
   </si>
   <si>
     <t>Nairobi</t>
+  </si>
+  <si>
+    <t>Cruise Line</t>
+  </si>
+  <si>
+    <t>Cruise Ship</t>
+  </si>
+  <si>
+    <t>Norwegian Cruise Line</t>
+  </si>
+  <si>
+    <t>Norwegian Epic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,18 +89,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -410,130 +376,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{27DD515B-791F-464B-93B7-A87C5826058F}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{6216C40C-8619-4583-A64B-5A1ACFF1EFF1}"/>
-  </hyperlinks>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87031940-51BD-4BD1-9AA8-D7723ED59C2F}">
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F29373-B20E-4CD5-8B0B-B41C4E1609FC}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
+      <c r="A2" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6164E875-B5E3-48CA-AA19-B4BC019A50AD}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32102D69-645A-4640-A840-44DD827D8ECD}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>